<commit_message>
Testing of first iteration 1
Completed first iteration testing
</commit_message>
<xml_diff>
--- a/Iteration-1/testing-plan-1.xlsx
+++ b/Iteration-1/testing-plan-1.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26221"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Taylor\Documents\Psychology\Psychology\Iteration-1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Test #</t>
   </si>
@@ -82,6 +87,30 @@
   </si>
   <si>
     <t>The user received a push notification at the end of the day</t>
+  </si>
+  <si>
+    <t>Actual Outcome</t>
+  </si>
+  <si>
+    <t>The initiative assessment successfully opened upon clicking 'Take Initiative Assessment' in the application</t>
+  </si>
+  <si>
+    <t>Inside the actual initiative assessment, the user is able to successfully input their answers to each question. The user can successfully submit their assessment by selecting 'submit' and seeing a dialog box open that says 'Your data was submitted'</t>
+  </si>
+  <si>
+    <t>The app does not send a push notification to the user at the end of the day. However, the end of day assessment was successfully created and can be taken by the user manually through the home page of the app</t>
+  </si>
+  <si>
+    <t>The app does not send push notifications to the user approximately 5x throughout the day. However, the random assessment was successfully created and can be taken by the user manually through the home page of the app</t>
+  </si>
+  <si>
+    <t>Success!</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Not fully working yet</t>
   </si>
 </sst>
 </file>
@@ -194,17 +223,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -228,9 +251,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -500,7 +541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -508,104 +549,136 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="12"/>
-    <col min="2" max="2" width="19.1640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="31" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="10"/>
+    <col min="2" max="2" width="21.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="11" customFormat="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="12" t="s">
         <v>12</v>
       </c>
+      <c r="F2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="70.5" customHeight="1">
-      <c r="A3" s="4">
+    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="F3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="42">
-      <c r="A4" s="4">
+    <row r="4" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="F4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="42">
-      <c r="A5" s="4">
+    <row r="5" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>